<commit_message>
Finitos2, Taller 2 2022b
</commit_message>
<xml_diff>
--- a/codigo/repaso_matricial/general_2D/portico_enlaces_rigidos.xlsx
+++ b/codigo/repaso_matricial/general_2D/portico_enlaces_rigidos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="45">
   <si>
     <t xml:space="preserve">nodo</t>
   </si>
@@ -576,9 +576,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -588,7 +588,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10222920" cy="9514080"/>
+          <a:ext cx="10252800" cy="9513360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -621,9 +621,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -633,7 +633,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10222920" cy="9514080"/>
+          <a:ext cx="10252800" cy="9513360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -671,9 +671,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>682920</xdr:colOff>
+      <xdr:colOff>682200</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -683,7 +683,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10161720" cy="9513720"/>
+          <a:ext cx="10186560" cy="9513000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -716,9 +716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>682920</xdr:colOff>
+      <xdr:colOff>682200</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -728,7 +728,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10161720" cy="9513720"/>
+          <a:ext cx="10186560" cy="9513000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -766,9 +766,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -778,7 +778,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10222920" cy="9513720"/>
+          <a:ext cx="10252800" cy="9513000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -811,9 +811,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -823,7 +823,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10222920" cy="9513720"/>
+          <a:ext cx="10252800" cy="9513000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -856,9 +856,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -868,7 +868,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10222920" cy="9513720"/>
+          <a:ext cx="10252800" cy="9513000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -901,9 +901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -913,7 +913,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10222920" cy="9513720"/>
+          <a:ext cx="10252800" cy="9513000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -951,9 +951,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -963,7 +963,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10222920" cy="9514080"/>
+          <a:ext cx="10252800" cy="9513360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -996,9 +996,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282960</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1008,7 +1008,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10222920" cy="9514080"/>
+          <a:ext cx="10252800" cy="9513360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1046,7 +1046,7 @@
       <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1790,11 +1790,11 @@
   </sheetPr>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E61" activeCellId="0" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.92"/>
   </cols>
@@ -2917,7 +2917,7 @@
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
   </cols>
@@ -3087,10 +3087,10 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I38" activeCellId="0" sqref="I38"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3126,6 +3126,9 @@
       <c r="E2" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -3143,6 +3146,9 @@
       <c r="E3" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -3160,6 +3166,9 @@
       <c r="E4" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -3177,6 +3186,9 @@
       <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -3194,6 +3206,9 @@
       <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -3211,6 +3226,9 @@
       <c r="E7" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F7" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -3228,6 +3246,9 @@
       <c r="E8" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -3245,6 +3266,9 @@
       <c r="E9" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F9" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -3261,6 +3285,9 @@
       </c>
       <c r="E10" s="4" t="n">
         <v>0</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,10 +3301,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,6 +3326,9 @@
       <c r="E12" s="4" t="n">
         <v>-20</v>
       </c>
+      <c r="F12" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -3308,10 +3341,13 @@
         <v>0</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E13" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3325,10 +3361,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,6 +3386,9 @@
       <c r="E15" s="4" t="n">
         <v>-20</v>
       </c>
+      <c r="F15" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -3359,10 +3401,13 @@
         <v>0</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3381,6 +3426,9 @@
       <c r="E17" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F17" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -3398,6 +3446,9 @@
       <c r="E18" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F18" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -3415,6 +3466,9 @@
       <c r="E19" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F19" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -3432,6 +3486,9 @@
       <c r="E20" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F20" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -3449,6 +3506,9 @@
       <c r="E21" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F21" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -3466,6 +3526,9 @@
       <c r="E22" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F22" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -3483,6 +3546,9 @@
       <c r="E23" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F23" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -3500,6 +3566,9 @@
       <c r="E24" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F24" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -3517,6 +3586,9 @@
       <c r="E25" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F25" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -3529,10 +3601,13 @@
         <v>0</v>
       </c>
       <c r="D26" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E26" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3551,6 +3626,9 @@
       <c r="E27" s="4" t="n">
         <v>-20</v>
       </c>
+      <c r="F27" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -3563,10 +3641,13 @@
         <v>0</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E28" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,10 +3661,13 @@
         <v>0</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E29" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3602,6 +3686,9 @@
       <c r="E30" s="4" t="n">
         <v>-20</v>
       </c>
+      <c r="F30" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -3614,10 +3701,13 @@
         <v>0</v>
       </c>
       <c r="D31" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E31" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,6 +3726,9 @@
       <c r="E32" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F32" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -3653,6 +3746,9 @@
       <c r="E33" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F33" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -3670,6 +3766,9 @@
       <c r="E34" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F34" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -3687,6 +3786,9 @@
       <c r="E35" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F35" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -3704,6 +3806,9 @@
       <c r="E36" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F36" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -3721,6 +3826,9 @@
       <c r="E37" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F37" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -3738,6 +3846,9 @@
       <c r="E38" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F38" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -3755,6 +3866,9 @@
       <c r="E39" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F39" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -3772,6 +3886,9 @@
       <c r="E40" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F40" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -3784,10 +3901,13 @@
         <v>0</v>
       </c>
       <c r="D41" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E41" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,6 +3926,9 @@
       <c r="E42" s="4" t="n">
         <v>-20</v>
       </c>
+      <c r="F42" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -3818,10 +3941,13 @@
         <v>0</v>
       </c>
       <c r="D43" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E43" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3835,10 +3961,13 @@
         <v>0</v>
       </c>
       <c r="D44" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E44" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3857,6 +3986,9 @@
       <c r="E45" s="4" t="n">
         <v>-20</v>
       </c>
+      <c r="F45" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -3869,10 +4001,13 @@
         <v>0</v>
       </c>
       <c r="D46" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E46" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,6 +4026,9 @@
       <c r="E47" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F47" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -3908,6 +4046,9 @@
       <c r="E48" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F48" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -3925,6 +4066,9 @@
       <c r="E49" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F49" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -3942,6 +4086,9 @@
       <c r="E50" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F50" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -3959,6 +4106,9 @@
       <c r="E51" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F51" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -3976,6 +4126,9 @@
       <c r="E52" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F52" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -3993,6 +4146,9 @@
       <c r="E53" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F53" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -4010,6 +4166,9 @@
       <c r="E54" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F54" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -4027,6 +4186,9 @@
       <c r="E55" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="F55" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -4039,10 +4201,13 @@
         <v>0</v>
       </c>
       <c r="D56" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E56" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4061,6 +4226,9 @@
       <c r="E57" s="4" t="n">
         <v>-20</v>
       </c>
+      <c r="F57" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -4073,10 +4241,13 @@
         <v>0</v>
       </c>
       <c r="D58" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E58" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4090,10 +4261,13 @@
         <v>0</v>
       </c>
       <c r="D59" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E59" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4112,6 +4286,9 @@
       <c r="E60" s="4" t="n">
         <v>-20</v>
       </c>
+      <c r="F60" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -4124,10 +4301,13 @@
         <v>0</v>
       </c>
       <c r="D61" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="E61" s="4" t="n">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4150,11 +4330,11 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4175,7 +4355,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4219,10 +4399,10 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
@@ -4301,11 +4481,11 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
@@ -4323,12 +4503,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4382,10 +4562,10 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>